<commit_message>
- Sony: fixed incorrect checksum error for Android based TVs which use CR+LF as line separators (normally only LF is used)
- Philips: show info that it may be necessary to unplug and reboot the TV after the import
- Philips ChannelMap_45: show info when there are checksum errors, which indicate that TV's internal list is broken
  and a rescan is required in order to properly export/import the list.
</commit_message>
<xml_diff>
--- a/source/Translation.xlsx
+++ b/source/Translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\ChanSort\Source\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA024CA3-56A8-4543-B196-A98F809ADF76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91340C08-CD88-4FE8-9594-5C787392737E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36750" yWindow="2865" windowWidth="36330" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ResXResourceManager" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8441" uniqueCount="2729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8579" uniqueCount="2747">
   <si>
     <t>Project</t>
   </si>
@@ -8389,7 +8389,15 @@
 - Provider: MUST be None/Other (do NOT select your cable provider or Astra 19.2E)
 - Blindscan: MUST be selected
 - Network search: optional (can be selected)
-Your TV will show a broken list if these steps are not followed!</t>
+Your TV will not process the list correctly if these steps are not followed!</t>
+  </si>
+  <si>
+    <t>!!! ACHTUNG !!!
+LG Senderlisten können NUR DANN vom Fernseher eingelesen werden, wenn bestimmte Optionen bei der Sendersuche gewählt wurden:
+- Anbieter: MUSS "Keiner" gewählt werden
+- Blindsuche: MUSS ausgewählt sein
+- Netzwerksuche: kann ausgewählt werden
+Ihr Fernseher wird die Senderliste nicht korrekt verarbeiten, wenn diese Schritte nicht befolgt wurden!</t>
   </si>
   <si>
     <t>LG_BlindscanInfo_OpenWebpage</t>
@@ -8398,10 +8406,28 @@
     <t>Read information about webOS 5 support on github.com</t>
   </si>
   <si>
+    <t>Webseite mit Infos zu webOS Unterstützung öffnen</t>
+  </si>
+  <si>
     <t>LG_BlindscanInfo_Continue</t>
   </si>
   <si>
+    <t>I searched for channels as described above</t>
+  </si>
+  <si>
+    <t>Ich habe die Sendersuche wie oben beschrieben durchgeführt</t>
+  </si>
+  <si>
     <t>LG_BlindscanInfo_Cancel</t>
+  </si>
+  <si>
+    <t>LG_BlindscanInfo_Rejected</t>
+  </si>
+  <si>
+    <t>Loading process was canceled</t>
+  </si>
+  <si>
+    <t>Ladevorgang wurde abgebrochen</t>
   </si>
   <si>
     <t>ChanSort.Loader.Hisense</t>
@@ -8469,10 +8495,57 @@
     <t>Kanal bulunamadı</t>
   </si>
   <si>
-    <t>I searched for channels as described above</t>
-  </si>
-  <si>
-    <t>Ich habe die Sendersuche wie oben beschrieben durchgeführt</t>
+    <t>ChanSort.Loader.Philips</t>
+  </si>
+  <si>
+    <t>InfoRestartAfterImport</t>
+  </si>
+  <si>
+    <t>INFO: After importing the list back in your TV, unplug it and plug it back in after a few seconds.</t>
+  </si>
+  <si>
+    <t>InfoIgnoreImportError</t>
+  </si>
+  <si>
+    <t>The TV may incorrectly show that the import failed, but that can be ignored.</t>
+  </si>
+  <si>
+    <t>WarningChecksumErrorMsg</t>
+  </si>
+  <si>
+    <t>WarningChechsumErrorIgnore</t>
+  </si>
+  <si>
+    <t>Ignore the error and edit the list anyway</t>
+  </si>
+  <si>
+    <t>INFO: Bitte schalten Sie Ihren Fernseher nach dem Import aus, ziehen den Netzstecker und stecken ihn nach einigen Sekunden wieder an.</t>
+  </si>
+  <si>
+    <t>Ihr Fernseher zeigt eventuell eine Falschmeldung, dass der Import fehlschlug. Dies kann ignoriert werden.</t>
+  </si>
+  <si>
+    <t>Fehler ignorieren und Datei trotzdem bearbeiten</t>
+  </si>
+  <si>
+    <t>WARNUNG: Beim Laden der Liste wurden Prüfsummenfehler festgestellt!
+Es gibt 2 typische Ursachen für dieses Problem:
+- Die interne Senderliste des Fernsehers ist beschädigt (z.B. nach einem Firmware-Update)
+   Dies kann durch einen neuen Suchlauf oder einen Reset behoben werden.
+   Exportieren Sie danach die Liste erneut und öffnen Sie sie in ChanSort.
+   Wenn Sie die Liste trotz Fehler bearbeiten und importieren, wird sie vermutlich nicht funktionieren.
+- Defekter USB-Stick (Speicherfehler oder inkomptibles Dateisystem)
+   Verwenden Sie nach Möglichkeit einen Stick &lt;= 16GB formatiert mit FAT32 (nicht NTFS oder exFAT)</t>
+  </si>
+  <si>
+    <t>WARNING: There were checksum errors in the loaded list!
+There are 2 situations how this can happen:
+- TV's internal channel list is corrupted (e.g. after a firmware update)
+   This can be solved by running a new channel scan or resetting the TV.
+   After that export the list again and open it with ChanSort.
+   Trying to edit and import the currently broken file can lead to unexpected behavior of the TV.
+- Bad USB-Stick (bad memory cells or incompatible file format)
+   Try using a Stick &lt;= 16GB formatted with FAT32 (not NTFS nor exFAT)</t>
   </si>
 </sst>
 </file>
@@ -8508,11 +8581,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8827,16 +8904,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W367"/>
+  <dimension ref="A1:W373"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A362" workbookViewId="0">
-      <selection activeCell="I364" sqref="I364"/>
+      <selection activeCell="F371" sqref="F371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -34496,7 +34572,7 @@
         <v>4</v>
       </c>
       <c r="I362" t="s">
-        <v>4</v>
+        <v>2706</v>
       </c>
       <c r="J362" t="s">
         <v>4</v>
@@ -34549,13 +34625,13 @@
         <v>2646</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>2706</v>
+        <v>2707</v>
       </c>
       <c r="D363" t="s">
         <v>4</v>
       </c>
       <c r="E363" t="s">
-        <v>2707</v>
+        <v>2708</v>
       </c>
       <c r="F363" t="s">
         <v>4</v>
@@ -34567,7 +34643,7 @@
         <v>4</v>
       </c>
       <c r="I363" t="s">
-        <v>4</v>
+        <v>2709</v>
       </c>
       <c r="J363" t="s">
         <v>4</v>
@@ -34620,13 +34696,13 @@
         <v>2646</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>2708</v>
+        <v>2710</v>
       </c>
       <c r="D364" t="s">
         <v>4</v>
       </c>
       <c r="E364" t="s">
-        <v>2727</v>
+        <v>2711</v>
       </c>
       <c r="F364" t="s">
         <v>4</v>
@@ -34638,7 +34714,7 @@
         <v>4</v>
       </c>
       <c r="I364" t="s">
-        <v>2728</v>
+        <v>2712</v>
       </c>
       <c r="J364" t="s">
         <v>4</v>
@@ -34691,7 +34767,7 @@
         <v>2646</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>2709</v>
+        <v>2713</v>
       </c>
       <c r="D365" t="s">
         <v>4</v>
@@ -34756,19 +34832,19 @@
     </row>
     <row r="366" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>2710</v>
+        <v>2443</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>2424</v>
+        <v>2646</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>2711</v>
+        <v>2714</v>
       </c>
       <c r="D366" t="s">
         <v>4</v>
       </c>
       <c r="E366" t="s">
-        <v>2712</v>
+        <v>2715</v>
       </c>
       <c r="F366" t="s">
         <v>4</v>
@@ -34780,25 +34856,25 @@
         <v>4</v>
       </c>
       <c r="I366" t="s">
-        <v>2713</v>
+        <v>2716</v>
       </c>
       <c r="J366" t="s">
         <v>4</v>
       </c>
       <c r="K366" t="s">
-        <v>2714</v>
+        <v>4</v>
       </c>
       <c r="L366" t="s">
         <v>4</v>
       </c>
       <c r="M366" t="s">
-        <v>2715</v>
+        <v>4</v>
       </c>
       <c r="N366" t="s">
         <v>4</v>
       </c>
       <c r="O366" t="s">
-        <v>2716</v>
+        <v>4</v>
       </c>
       <c r="P366" t="s">
         <v>4</v>
@@ -34810,7 +34886,7 @@
         <v>4</v>
       </c>
       <c r="S366" t="s">
-        <v>2717</v>
+        <v>4</v>
       </c>
       <c r="T366" t="s">
         <v>4</v>
@@ -34822,78 +34898,504 @@
         <v>4</v>
       </c>
       <c r="W366" t="s">
-        <v>2718</v>
+        <v>4</v>
       </c>
     </row>
     <row r="367" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>2710</v>
+        <v>2717</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>2424</v>
       </c>
       <c r="C367" s="1" t="s">
+        <v>2718</v>
+      </c>
+      <c r="D367" t="s">
+        <v>4</v>
+      </c>
+      <c r="E367" t="s">
         <v>2719</v>
       </c>
-      <c r="D367" t="s">
-        <v>4</v>
-      </c>
-      <c r="E367" t="s">
+      <c r="F367" t="s">
+        <v>4</v>
+      </c>
+      <c r="G367" t="s">
+        <v>4</v>
+      </c>
+      <c r="H367" t="s">
+        <v>4</v>
+      </c>
+      <c r="I367" t="s">
         <v>2720</v>
       </c>
-      <c r="F367" t="s">
-        <v>4</v>
-      </c>
-      <c r="G367" t="s">
-        <v>4</v>
-      </c>
-      <c r="H367" t="s">
-        <v>4</v>
-      </c>
-      <c r="I367" t="s">
+      <c r="J367" t="s">
+        <v>4</v>
+      </c>
+      <c r="K367" t="s">
         <v>2721</v>
       </c>
-      <c r="J367" t="s">
-        <v>4</v>
-      </c>
-      <c r="K367" t="s">
+      <c r="L367" t="s">
+        <v>4</v>
+      </c>
+      <c r="M367" t="s">
         <v>2722</v>
       </c>
-      <c r="L367" t="s">
-        <v>4</v>
-      </c>
-      <c r="M367" t="s">
+      <c r="N367" t="s">
+        <v>4</v>
+      </c>
+      <c r="O367" t="s">
         <v>2723</v>
       </c>
-      <c r="N367" t="s">
-        <v>4</v>
-      </c>
-      <c r="O367" t="s">
+      <c r="P367" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q367" t="s">
+        <v>4</v>
+      </c>
+      <c r="R367" t="s">
+        <v>4</v>
+      </c>
+      <c r="S367" t="s">
         <v>2724</v>
       </c>
-      <c r="P367" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q367" t="s">
-        <v>4</v>
-      </c>
-      <c r="R367" t="s">
-        <v>4</v>
-      </c>
-      <c r="S367" t="s">
+      <c r="T367" t="s">
+        <v>4</v>
+      </c>
+      <c r="U367" t="s">
+        <v>4</v>
+      </c>
+      <c r="V367" t="s">
+        <v>4</v>
+      </c>
+      <c r="W367" t="s">
         <v>2725</v>
       </c>
-      <c r="T367" t="s">
-        <v>4</v>
-      </c>
-      <c r="U367" t="s">
-        <v>4</v>
-      </c>
-      <c r="V367" t="s">
-        <v>4</v>
-      </c>
-      <c r="W367" t="s">
+    </row>
+    <row r="368" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A368" s="1" t="s">
+        <v>2717</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C368" s="1" t="s">
         <v>2726</v>
+      </c>
+      <c r="D368" t="s">
+        <v>4</v>
+      </c>
+      <c r="E368" t="s">
+        <v>2727</v>
+      </c>
+      <c r="F368" t="s">
+        <v>4</v>
+      </c>
+      <c r="G368" t="s">
+        <v>4</v>
+      </c>
+      <c r="H368" t="s">
+        <v>4</v>
+      </c>
+      <c r="I368" t="s">
+        <v>2728</v>
+      </c>
+      <c r="J368" t="s">
+        <v>4</v>
+      </c>
+      <c r="K368" t="s">
+        <v>2729</v>
+      </c>
+      <c r="L368" t="s">
+        <v>4</v>
+      </c>
+      <c r="M368" t="s">
+        <v>2730</v>
+      </c>
+      <c r="N368" t="s">
+        <v>4</v>
+      </c>
+      <c r="O368" t="s">
+        <v>2731</v>
+      </c>
+      <c r="P368" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q368" t="s">
+        <v>4</v>
+      </c>
+      <c r="R368" t="s">
+        <v>4</v>
+      </c>
+      <c r="S368" t="s">
+        <v>2732</v>
+      </c>
+      <c r="T368" t="s">
+        <v>4</v>
+      </c>
+      <c r="U368" t="s">
+        <v>4</v>
+      </c>
+      <c r="V368" t="s">
+        <v>4</v>
+      </c>
+      <c r="W368" t="s">
+        <v>2733</v>
+      </c>
+    </row>
+    <row r="369" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A369" s="1" t="s">
+        <v>2734</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>2735</v>
+      </c>
+      <c r="D369" t="s">
+        <v>4</v>
+      </c>
+      <c r="E369" t="s">
+        <v>2736</v>
+      </c>
+      <c r="F369" t="s">
+        <v>4</v>
+      </c>
+      <c r="G369" t="s">
+        <v>4</v>
+      </c>
+      <c r="H369" t="s">
+        <v>4</v>
+      </c>
+      <c r="I369" t="s">
+        <v>2742</v>
+      </c>
+      <c r="J369" t="s">
+        <v>4</v>
+      </c>
+      <c r="K369" t="s">
+        <v>4</v>
+      </c>
+      <c r="L369" t="s">
+        <v>4</v>
+      </c>
+      <c r="M369" t="s">
+        <v>4</v>
+      </c>
+      <c r="N369" t="s">
+        <v>4</v>
+      </c>
+      <c r="O369" t="s">
+        <v>4</v>
+      </c>
+      <c r="P369" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q369" t="s">
+        <v>4</v>
+      </c>
+      <c r="R369" t="s">
+        <v>4</v>
+      </c>
+      <c r="S369" t="s">
+        <v>4</v>
+      </c>
+      <c r="T369" t="s">
+        <v>4</v>
+      </c>
+      <c r="U369" t="s">
+        <v>4</v>
+      </c>
+      <c r="V369" t="s">
+        <v>4</v>
+      </c>
+      <c r="W369" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="370" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A370" s="1" t="s">
+        <v>2734</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>2737</v>
+      </c>
+      <c r="D370" t="s">
+        <v>4</v>
+      </c>
+      <c r="E370" t="s">
+        <v>2738</v>
+      </c>
+      <c r="F370" t="s">
+        <v>4</v>
+      </c>
+      <c r="G370" t="s">
+        <v>4</v>
+      </c>
+      <c r="H370" t="s">
+        <v>4</v>
+      </c>
+      <c r="I370" t="s">
+        <v>2743</v>
+      </c>
+      <c r="J370" t="s">
+        <v>4</v>
+      </c>
+      <c r="K370" t="s">
+        <v>4</v>
+      </c>
+      <c r="L370" t="s">
+        <v>4</v>
+      </c>
+      <c r="M370" t="s">
+        <v>4</v>
+      </c>
+      <c r="N370" t="s">
+        <v>4</v>
+      </c>
+      <c r="O370" t="s">
+        <v>4</v>
+      </c>
+      <c r="P370" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q370" t="s">
+        <v>4</v>
+      </c>
+      <c r="R370" t="s">
+        <v>4</v>
+      </c>
+      <c r="S370" t="s">
+        <v>4</v>
+      </c>
+      <c r="T370" t="s">
+        <v>4</v>
+      </c>
+      <c r="U370" t="s">
+        <v>4</v>
+      </c>
+      <c r="V370" t="s">
+        <v>4</v>
+      </c>
+      <c r="W370" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="371" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A371" s="1" t="s">
+        <v>2734</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>2739</v>
+      </c>
+      <c r="D371" t="s">
+        <v>4</v>
+      </c>
+      <c r="E371" s="2" t="s">
+        <v>2746</v>
+      </c>
+      <c r="F371" t="s">
+        <v>4</v>
+      </c>
+      <c r="G371" t="s">
+        <v>4</v>
+      </c>
+      <c r="H371" t="s">
+        <v>4</v>
+      </c>
+      <c r="I371" s="2" t="s">
+        <v>2745</v>
+      </c>
+      <c r="J371" t="s">
+        <v>4</v>
+      </c>
+      <c r="K371" t="s">
+        <v>4</v>
+      </c>
+      <c r="L371" t="s">
+        <v>4</v>
+      </c>
+      <c r="M371" t="s">
+        <v>4</v>
+      </c>
+      <c r="N371" t="s">
+        <v>4</v>
+      </c>
+      <c r="O371" t="s">
+        <v>4</v>
+      </c>
+      <c r="P371" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q371" t="s">
+        <v>4</v>
+      </c>
+      <c r="R371" t="s">
+        <v>4</v>
+      </c>
+      <c r="S371" t="s">
+        <v>4</v>
+      </c>
+      <c r="T371" t="s">
+        <v>4</v>
+      </c>
+      <c r="U371" t="s">
+        <v>4</v>
+      </c>
+      <c r="V371" t="s">
+        <v>4</v>
+      </c>
+      <c r="W371" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="372" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A372" s="1" t="s">
+        <v>2734</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>2740</v>
+      </c>
+      <c r="D372" t="s">
+        <v>4</v>
+      </c>
+      <c r="E372" t="s">
+        <v>2741</v>
+      </c>
+      <c r="F372" t="s">
+        <v>4</v>
+      </c>
+      <c r="G372" t="s">
+        <v>4</v>
+      </c>
+      <c r="H372" t="s">
+        <v>4</v>
+      </c>
+      <c r="I372" t="s">
+        <v>2744</v>
+      </c>
+      <c r="J372" t="s">
+        <v>4</v>
+      </c>
+      <c r="K372" t="s">
+        <v>4</v>
+      </c>
+      <c r="L372" t="s">
+        <v>4</v>
+      </c>
+      <c r="M372" t="s">
+        <v>4</v>
+      </c>
+      <c r="N372" t="s">
+        <v>4</v>
+      </c>
+      <c r="O372" t="s">
+        <v>4</v>
+      </c>
+      <c r="P372" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q372" t="s">
+        <v>4</v>
+      </c>
+      <c r="R372" t="s">
+        <v>4</v>
+      </c>
+      <c r="S372" t="s">
+        <v>4</v>
+      </c>
+      <c r="T372" t="s">
+        <v>4</v>
+      </c>
+      <c r="U372" t="s">
+        <v>4</v>
+      </c>
+      <c r="V372" t="s">
+        <v>4</v>
+      </c>
+      <c r="W372" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="373" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A373" s="1" t="s">
+        <v>2734</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D373" t="s">
+        <v>4</v>
+      </c>
+      <c r="E373" t="s">
+        <v>118</v>
+      </c>
+      <c r="F373" t="s">
+        <v>4</v>
+      </c>
+      <c r="G373" t="s">
+        <v>119</v>
+      </c>
+      <c r="H373" t="s">
+        <v>4</v>
+      </c>
+      <c r="I373" t="s">
+        <v>120</v>
+      </c>
+      <c r="J373" t="s">
+        <v>4</v>
+      </c>
+      <c r="K373" t="s">
+        <v>121</v>
+      </c>
+      <c r="L373" t="s">
+        <v>4</v>
+      </c>
+      <c r="M373" t="s">
+        <v>122</v>
+      </c>
+      <c r="N373" t="s">
+        <v>4</v>
+      </c>
+      <c r="O373" t="s">
+        <v>123</v>
+      </c>
+      <c r="P373" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q373" t="s">
+        <v>4</v>
+      </c>
+      <c r="R373" t="s">
+        <v>4</v>
+      </c>
+      <c r="S373" t="s">
+        <v>125</v>
+      </c>
+      <c r="T373" t="s">
+        <v>4</v>
+      </c>
+      <c r="U373" t="s">
+        <v>4</v>
+      </c>
+      <c r="V373" t="s">
+        <v>4</v>
+      </c>
+      <c r="W373" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Sony: Files with incorrect checksum are no longer rejected. Information about a bad checksum is visible
  unter File / File Information. (The TV seems to ignore bad checksums during the import and the official
  Sony PC Editor ignores bad checksums and write incorrect ones, depending on the file format version)
- Updated Hungarian translation. Thanks to efi99 on Github!
- Minor cleanup amongst translation (setting @Invariant for constant strings and unifying "..." in menu items that open a new dialog)
</commit_message>
<xml_diff>
--- a/source/Translation.xlsx
+++ b/source/Translation.xlsx
@@ -320,7 +320,7 @@
       </x:c>
       <x:c r="G3" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">http://github.com/PredatH0r/ChanSort</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="H3" t="inlineStr">
@@ -340,7 +340,7 @@
       </x:c>
       <x:c r="K3" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">http://github.com/PredatH0r/ChanSort</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="L3" t="inlineStr">
@@ -350,7 +350,7 @@
       </x:c>
       <x:c r="M3" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">http://github.com/PredatH0r/ChanSort</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="N3" t="inlineStr">
@@ -360,7 +360,7 @@
       </x:c>
       <x:c r="O3" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">http://github.com/PredatH0r/ChanSort</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="P3" t="inlineStr">
@@ -400,7 +400,7 @@
       </x:c>
       <x:c r="W3" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">http://github.com/PredatH0r/ChanSort</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
     </x:row>
@@ -437,7 +437,7 @@
       </x:c>
       <x:c r="G4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">horst@beham.biz</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="H4" t="inlineStr">
@@ -457,7 +457,7 @@
       </x:c>
       <x:c r="K4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">horst@beham.biz</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="L4" t="inlineStr">
@@ -467,7 +467,7 @@
       </x:c>
       <x:c r="M4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">horst@beham.biz</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="N4" t="inlineStr">
@@ -477,7 +477,7 @@
       </x:c>
       <x:c r="O4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">horst@beham.biz</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="P4" t="inlineStr">
@@ -517,7 +517,7 @@
       </x:c>
       <x:c r="W4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">horst@beham.biz</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
     </x:row>
@@ -788,7 +788,7 @@
       </x:c>
       <x:c r="G7" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">GNU GPLv3</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="H7" t="inlineStr">
@@ -808,7 +808,7 @@
       </x:c>
       <x:c r="K7" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">GNU GPLv3</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="L7" t="inlineStr">
@@ -818,7 +818,7 @@
       </x:c>
       <x:c r="M7" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">GNU GPLv3</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="N7" t="inlineStr">
@@ -828,7 +828,7 @@
       </x:c>
       <x:c r="O7" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">GNU GPLv3</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="P7" t="inlineStr">
@@ -868,7 +868,7 @@
       </x:c>
       <x:c r="W7" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">GNU GPLv3</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
     </x:row>
@@ -1169,7 +1169,7 @@
       </x:c>
       <x:c r="M10" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Horst Beham</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="N10" t="inlineStr">
@@ -1510,7 +1510,7 @@
       </x:c>
       <x:c r="K13" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Seleccione una opción…</x:t>
+          <x:t xml:space="preserve">Seleccione una opción...</x:t>
         </x:is>
       </x:c>
       <x:c r="L13" t="inlineStr">
@@ -1520,7 +1520,7 @@
       </x:c>
       <x:c r="M13" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Válasszon egy műveletet…</x:t>
+          <x:t xml:space="preserve">Válasszon egy műveletet...</x:t>
         </x:is>
       </x:c>
       <x:c r="N13" t="inlineStr">
@@ -1570,7 +1570,7 @@
       </x:c>
       <x:c r="W13" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Bir eylem seçin…</x:t>
+          <x:t xml:space="preserve">Bir eylem seçin...</x:t>
         </x:is>
       </x:c>
     </x:row>
@@ -3743,7 +3743,7 @@
       </x:c>
       <x:c r="M32" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Egy csatorna keresése</x:t>
         </x:is>
       </x:c>
       <x:c r="N32" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </x:c>
       <x:c r="W36" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">TV veri dosyasını aç…</x:t>
+          <x:t xml:space="preserve">TV veri dosyasını aç...</x:t>
         </x:is>
       </x:c>
     </x:row>
@@ -4532,7 +4532,7 @@
       </x:c>
       <x:c r="G39" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Informace o souboru</x:t>
+          <x:t xml:space="preserve">Informace o souboru...</x:t>
         </x:is>
       </x:c>
       <x:c r="H39" t="inlineStr">
@@ -4552,7 +4552,7 @@
       </x:c>
       <x:c r="K39" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Archivo e información…</x:t>
+          <x:t xml:space="preserve">Archivo e información...</x:t>
         </x:is>
       </x:c>
       <x:c r="L39" t="inlineStr">
@@ -4612,7 +4612,7 @@
       </x:c>
       <x:c r="W39" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Dosya bilgisi</x:t>
+          <x:t xml:space="preserve">Dosya bilgisi...</x:t>
         </x:is>
       </x:c>
     </x:row>
@@ -4796,7 +4796,7 @@
       </x:c>
       <x:c r="M41" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Mentés m&amp;ásként</x:t>
+          <x:t xml:space="preserve">Mentés m&amp;ásként...</x:t>
         </x:is>
       </x:c>
       <x:c r="N41" t="inlineStr">
@@ -4963,7 +4963,7 @@
       </x:c>
       <x:c r="W42" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Referans listesinden düzen uygula…</x:t>
+          <x:t xml:space="preserve">Referans listesinden düzen uygula...</x:t>
         </x:is>
       </x:c>
     </x:row>
@@ -5254,7 +5254,7 @@
       </x:c>
       <x:c r="K45" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Exportar lista de Excel</x:t>
+          <x:t xml:space="preserve">Exportar lista de Excel...</x:t>
         </x:is>
       </x:c>
       <x:c r="L45" t="inlineStr">
@@ -5314,7 +5314,7 @@
       </x:c>
       <x:c r="W45" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Excel listesini dışa aktar…</x:t>
+          <x:t xml:space="preserve">Excel listesini dışa aktar...</x:t>
         </x:is>
       </x:c>
     </x:row>
@@ -5371,7 +5371,7 @@
       </x:c>
       <x:c r="K46" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">&amp;Imprimir</x:t>
+          <x:t xml:space="preserve">&amp;Imprimir...</x:t>
         </x:is>
       </x:c>
       <x:c r="L46" t="inlineStr">
@@ -5431,7 +5431,7 @@
       </x:c>
       <x:c r="W46" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Yazdır</x:t>
+          <x:t xml:space="preserve">Yazdır...</x:t>
         </x:is>
       </x:c>
     </x:row>
@@ -8540,7 +8540,7 @@
       </x:c>
       <x:c r="M73" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Osztott nézet</x:t>
         </x:is>
       </x:c>
       <x:c r="N73" t="inlineStr">
@@ -8657,7 +8657,7 @@
       </x:c>
       <x:c r="M74" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">&amp;Nyelv</x:t>
         </x:is>
       </x:c>
       <x:c r="N74" t="inlineStr">
@@ -8729,7 +8729,7 @@
       </x:c>
       <x:c r="D75" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E75" t="inlineStr">
@@ -8846,7 +8846,7 @@
       </x:c>
       <x:c r="D76" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E76" t="inlineStr">
@@ -8963,7 +8963,7 @@
       </x:c>
       <x:c r="D77" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E77" t="inlineStr">
@@ -9080,7 +9080,7 @@
       </x:c>
       <x:c r="D78" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E78" t="inlineStr">
@@ -9197,7 +9197,7 @@
       </x:c>
       <x:c r="D79" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E79" t="inlineStr">
@@ -9314,7 +9314,7 @@
       </x:c>
       <x:c r="D80" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E80" t="inlineStr">
@@ -9431,7 +9431,7 @@
       </x:c>
       <x:c r="D81" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E81" t="inlineStr">
@@ -9548,7 +9548,7 @@
       </x:c>
       <x:c r="D82" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E82" t="inlineStr">
@@ -9665,7 +9665,7 @@
       </x:c>
       <x:c r="D83" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E83" t="inlineStr">
@@ -9782,7 +9782,7 @@
       </x:c>
       <x:c r="D84" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E84" t="inlineStr">
@@ -10133,7 +10133,7 @@
       </x:c>
       <x:c r="D87" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E87" t="inlineStr">
@@ -10367,7 +10367,7 @@
       </x:c>
       <x:c r="D89" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E89" t="inlineStr">
@@ -10484,7 +10484,7 @@
       </x:c>
       <x:c r="D90" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E90" t="inlineStr">
@@ -11465,7 +11465,7 @@
       </x:c>
       <x:c r="M98" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Alaphelyzetbe állítás és újraindítás</x:t>
         </x:is>
       </x:c>
       <x:c r="N98" t="inlineStr">
@@ -11582,7 +11582,7 @@
       </x:c>
       <x:c r="M99" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Töröl minden egyéni beállítást és újraindítja a programot</x:t>
         </x:is>
       </x:c>
       <x:c r="N99" t="inlineStr">
@@ -13526,7 +13526,7 @@
       </x:c>
       <x:c r="D116" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E116" t="inlineStr">
@@ -13643,7 +13643,7 @@
       </x:c>
       <x:c r="D117" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E117" t="inlineStr">
@@ -13760,7 +13760,7 @@
       </x:c>
       <x:c r="D118" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E118" t="inlineStr">
@@ -13877,7 +13877,7 @@
       </x:c>
       <x:c r="D119" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E119" t="inlineStr">
@@ -13994,7 +13994,7 @@
       </x:c>
       <x:c r="D120" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E120" t="inlineStr">
@@ -14380,7 +14380,7 @@
       </x:c>
       <x:c r="K123" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Sitio Web de ChanSort…</x:t>
+          <x:t xml:space="preserve">Sitio Web de ChanSort...</x:t>
         </x:is>
       </x:c>
       <x:c r="L123" t="inlineStr">
@@ -14440,7 +14440,7 @@
       </x:c>
       <x:c r="W123" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">ChanSort sayfası</x:t>
+          <x:t xml:space="preserve">ChanSort sayfası...</x:t>
         </x:is>
       </x:c>
     </x:row>
@@ -15749,7 +15749,7 @@
       </x:c>
       <x:c r="D135" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">@Invariant</x:t>
         </x:is>
       </x:c>
       <x:c r="E135" t="inlineStr">
@@ -15764,7 +15764,7 @@
       </x:c>
       <x:c r="G135" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">\d{1,4}</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="H135" t="inlineStr">
@@ -15784,7 +15784,7 @@
       </x:c>
       <x:c r="K135" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">\d{1,4}</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="L135" t="inlineStr">
@@ -15794,7 +15794,7 @@
       </x:c>
       <x:c r="M135" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">\d{1,4}</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="N135" t="inlineStr">
@@ -15804,7 +15804,7 @@
       </x:c>
       <x:c r="O135" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">\d{1,4}</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="P135" t="inlineStr">
@@ -15824,7 +15824,7 @@
       </x:c>
       <x:c r="S135" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">\d{1,4}</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
       <x:c r="T135" t="inlineStr">
@@ -15844,7 +15844,7 @@
       </x:c>
       <x:c r="W135" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">\d{1,4}</x:t>
+          <x:t xml:space="preserve"/>
         </x:is>
       </x:c>
     </x:row>
@@ -16028,7 +16028,7 @@
       </x:c>
       <x:c r="M137" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Csatorna keresése név alapján</x:t>
         </x:is>
       </x:c>
       <x:c r="N137" t="inlineStr">
@@ -18953,7 +18953,7 @@
       </x:c>
       <x:c r="M162" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Mozgassa a kijelölt csatornát lefelé</x:t>
+          <x:t xml:space="preserve">Mozgassa a kijelölt csatornákat lefelé</x:t>
         </x:is>
       </x:c>
       <x:c r="N162" t="inlineStr">
@@ -19187,7 +19187,7 @@
       </x:c>
       <x:c r="M164" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Mozgassa a kijelölt csatornát felfelé</x:t>
+          <x:t xml:space="preserve">Mozgassa a kijelölt csatornákat felfelé</x:t>
         </x:is>
       </x:c>
       <x:c r="N164" t="inlineStr">
@@ -24218,7 +24218,7 @@
       </x:c>
       <x:c r="M207" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Egy csatorna keresése</x:t>
         </x:is>
       </x:c>
       <x:c r="N207" t="inlineStr">
@@ -24335,7 +24335,7 @@
       </x:c>
       <x:c r="M208" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Csatorna keresése név alapján</x:t>
         </x:is>
       </x:c>
       <x:c r="N208" t="inlineStr">
@@ -24926,7 +24926,7 @@
       </x:c>
       <x:c r="M213" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">#N/A</x:t>
+          <x:t xml:space="preserve">Az összes jelenleg nem rendezett csatorna hozzáfűzése a lista végéhez</x:t>
         </x:is>
       </x:c>
       <x:c r="N213" t="inlineStr">
@@ -30758,7 +30758,7 @@
       </x:c>
       <x:c r="G263" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Ok</x:t>
         </x:is>
       </x:c>
       <x:c r="H263" t="inlineStr">
@@ -30768,7 +30768,7 @@
       </x:c>
       <x:c r="I263" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Ok</x:t>
         </x:is>
       </x:c>
       <x:c r="J263" t="inlineStr">
@@ -31735,7 +31735,7 @@
       </x:c>
       <x:c r="M271" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Alapértelmezett téme használata</x:t>
         </x:is>
       </x:c>
       <x:c r="N271" t="inlineStr">
@@ -33363,7 +33363,7 @@
       </x:c>
       <x:c r="K285" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Previsualizar…</x:t>
+          <x:t xml:space="preserve">Previsualizar...</x:t>
         </x:is>
       </x:c>
       <x:c r="L285" t="inlineStr">
@@ -41091,7 +41091,12 @@
       </x:c>
       <x:c r="M349" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">!!! FIGYELEM !!!
+Az LG csatornalistákat CSAK akkor lehet visszaimportálni a tévékészülékbe, ha a csatornakeresési folyamat során speciális beállítások voltak kiválasztva:
+- Szolgáltató: Nincs/Egyéb KELL (NE válasszon ki a kábelszolgáltatót vagy az Astra 19.2E -t)
+- Blindscan: ki KELL jelölni
+- Hálózati keresés: opcionális (kiválasztható)
+TV -je nem fogja megfelelően feldolgozni a listát, ha nem követi ezeket a lépéseket!</x:t>
         </x:is>
       </x:c>
       <x:c r="N349" t="inlineStr">
@@ -41208,7 +41213,7 @@
       </x:c>
       <x:c r="M350" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">A webOS5 támogatásáról szóló információkat olvassa el a github.com-on</x:t>
         </x:is>
       </x:c>
       <x:c r="N350" t="inlineStr">
@@ -41325,7 +41330,7 @@
       </x:c>
       <x:c r="M351" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">A csatorna keresés a fent leírtak szerint történt</x:t>
         </x:is>
       </x:c>
       <x:c r="N351" t="inlineStr">
@@ -41559,7 +41564,7 @@
       </x:c>
       <x:c r="M353" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">A betöltési folyamat leállítva</x:t>
         </x:is>
       </x:c>
       <x:c r="N353" t="inlineStr">
@@ -41924,7 +41929,7 @@
       </x:c>
       <x:c r="M356" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Lehet, hogy a TV hibásan mutatja, hogy az importálás sikertelen volt, de ezt figyelmen kívül lehet hagyni.</x:t>
         </x:is>
       </x:c>
       <x:c r="N356" t="inlineStr">
@@ -42041,7 +42046,7 @@
       </x:c>
       <x:c r="M357" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">INFORMÁCIÓ: Miután importálta a listát a TV -be, húzza ki a hálózati csatlakozót, majd néhány másodperc múlva csatlakoztassa újra.</x:t>
         </x:is>
       </x:c>
       <x:c r="N357" t="inlineStr">
@@ -42172,7 +42177,14 @@
       </x:c>
       <x:c r="M358" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">FIGYELEM: Ellenőrző összeg hibák voltak a betöltött listában!
+Ez két esetben fordul elő:
+- A TV belső csatornalistája sérült (pl. Firmware frissítés után)
+    Ez megoldható új csatornakeresés újrafuttatásával vagy a TV alaphelyzetbe állításával.
+    Ezt követően újra exportálja a listát, és nyissa meg a ChanSort segítségével.
+    A jelenleg meghibásodott fájl szerkesztésének és importálásának kísérlete a TV -készülék váratlan viselkedéséhez vezethet.
+- Hibás USB-stick (rossz memóriacellák vagy nem kompatibilis fájlformátum)
+    Próbáljon meg egy 16 GB-osnál nem nagyobb, FAT32 -es (nem NTFS és exFAT) formátumú pendrive-ot használni</x:t>
         </x:is>
       </x:c>
       <x:c r="N358" t="inlineStr">
@@ -42289,7 +42301,7 @@
       </x:c>
       <x:c r="M359" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Hiba figyelmenkívül hagyása és a lista szerkesztése</x:t>
         </x:is>
       </x:c>
       <x:c r="N359" t="inlineStr">

</xml_diff>